<commit_message>
Sprint 1 Burndown Chart mit Daten geupdated
</commit_message>
<xml_diff>
--- a/Gehweg-Parcours Sprint 1 Burndown Chart.xlsx
+++ b/Gehweg-Parcours Sprint 1 Burndown Chart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\etc\@eclipse\AB_Kaunas_Adrian_ORIG\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nick\OneDrive\Schule\Klasse 11\IT\Software\eclipse\Gehweg-Parcours\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BB40A2DA-E047-4692-858C-E7A00B2461D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4D42B9C-4323-43D2-B423-B2864FA4DDB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Gehweg-Parcours" sheetId="1" r:id="rId1"/>
@@ -277,13 +277,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>7</c:v>
                 </c:pt>
-                <c:pt idx="1">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -341,16 +341,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>7</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>7</c:v>
+                  <c:v>-1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1585,19 +1585,19 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.3984375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.3984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.3984375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.1328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.3984375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="16.44140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.44140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.44140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1610,7 +1610,7 @@
       </c>
       <c r="E1" s="7"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="7"/>
       <c r="B2" s="5" t="s">
         <v>3</v>
@@ -1625,67 +1625,77 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5">
         <f>SUM(B4:B6)</f>
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="5">
         <f>C3</f>
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <v>44699</v>
       </c>
       <c r="B4" s="2">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C4" s="5">
         <f>C3-B4</f>
-        <v>0</v>
-      </c>
-      <c r="D4" s="2"/>
+        <v>7</v>
+      </c>
+      <c r="D4" s="2">
+        <v>3</v>
+      </c>
       <c r="E4" s="5">
         <f>E3-D4</f>
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="6">
         <v>44701</v>
       </c>
-      <c r="B5" s="2"/>
+      <c r="B5" s="2">
+        <v>4</v>
+      </c>
       <c r="C5" s="5">
         <f>C4-B5</f>
-        <v>0</v>
-      </c>
-      <c r="D5" s="2"/>
+        <v>3</v>
+      </c>
+      <c r="D5" s="2">
+        <v>5</v>
+      </c>
       <c r="E5" s="5">
         <f>E4-D5</f>
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="6">
         <v>44715</v>
       </c>
-      <c r="B6" s="2"/>
+      <c r="B6" s="2">
+        <v>3</v>
+      </c>
       <c r="C6" s="5">
         <f t="shared" ref="C6:E6" si="0">C5-B6</f>
         <v>0</v>
       </c>
-      <c r="D6" s="2"/>
+      <c r="D6" s="2">
+        <v>3</v>
+      </c>
       <c r="E6" s="5">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>-1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="4"/>
     </row>
   </sheetData>

</xml_diff>